<commit_message>
added overall stats, willard
</commit_message>
<xml_diff>
--- a/Yearly Reports/2018/Willard/Willard Report.xlsx
+++ b/Yearly Reports/2018/Willard/Willard Report.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\GitHub\FitzFishing\Yearly Reports\2018\Willard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FCD30D-EB37-4906-A2A5-F6D7DCE97A02}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525CE243-B900-4AF8-801A-2C455D3FEDC6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AE8D5F39-7595-4FC6-A891-11E1A93D88B1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{AE8D5F39-7595-4FC6-A891-11E1A93D88B1}"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" r:id="rId1"/>
+    <sheet name="Overall Stats" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Lake/Pond</t>
   </si>
@@ -229,6 +230,1942 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>total</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> species caught</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="27000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="88000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="flat">
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="30000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Overall Stats'!$A$2:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>C. Catfish</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SM. Bass</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Overall Stats'!$A$3:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-05CC-47CE-B704-BBA7FF27F50B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="84"/>
+        <c:gapDepth val="53"/>
+        <c:shape val="box"/>
+        <c:axId val="101034528"/>
+        <c:axId val="2102033232"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="101034528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2102033232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2102033232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="101034528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:tint val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PERCENT</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> SPECIES CAUGHT</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Overall Stats'!$A$5:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>C. Catfish</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SM. Bass</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Overall Stats'!$A$6:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E083-4660-B1D0-85BD5DC5BEFE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="291">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:tint val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="30000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="30000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="88000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="88000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg2">
+          <a:lumMod val="75000"/>
+          <a:alpha val="27000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="0" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="268">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E21B3BF5-8FD4-40BD-914F-B1AC01511C90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A843546-9D5B-4C77-8894-F16C8B61F360}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -528,7 +2465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF203B8-BFD1-44BC-8BFD-659ECFF9578C}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -606,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -620,8 +2557,14 @@
       <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="F5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
@@ -629,25 +2572,27 @@
         <f>SUM(D4:D5)</f>
         <v>2</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
+      <c r="F6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="11">
         <v>2</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>7</v>
+      <c r="F7">
+        <f>SUM(F4/$D$6*100)</f>
+        <v>50</v>
+      </c>
+      <c r="G7">
+        <f>SUM(G4/$D$6*100)</f>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -657,22 +2602,116 @@
       <c r="D8" s="11">
         <f>AVERAGE(D4:D5)</f>
         <v>1</v>
-      </c>
-      <c r="F8">
-        <f>SUM(F4/$D$6*100)</f>
-        <v>50</v>
-      </c>
-      <c r="G8">
-        <f>SUM(G4/$D$6*100)</f>
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDE7405-D35D-40BA-960D-7EDFE6E4F7AD}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <f>SUM('2018'!F4)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <f>SUM('2018'!G4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>SUM(A3/$B$8*100)</f>
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <f>SUM(B3/$B$8*100)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="11">
+        <f>SUM('2018'!D6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="11">
+        <f>SUM(B8/B9)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>